<commit_message>
update script leaf growth
</commit_message>
<xml_diff>
--- a/data/C3M42_leafGrowth.xlsx
+++ b/data/C3M42_leafGrowth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis/Documents/Encadrements/Stages/2021 - M2 - Benoit Berthet - Endopolyploidy/R_Git_PLASTENDO/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C877B121-AB20-AA4F-A6C9-8462D95327C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D0B7A-D93A-7E4D-8645-75635952A045}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2917,8 +2917,8 @@
   <dimension ref="A1:I1262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C171" sqref="C171"/>
+      <pane ySplit="1" topLeftCell="A659" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A664" sqref="A664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20758,7 +20758,7 @@
         <v>457</v>
       </c>
       <c r="B654" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C654" s="4" t="s">
         <v>401</v>
@@ -20785,7 +20785,7 @@
         <v>458</v>
       </c>
       <c r="B655" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C655" s="4" t="s">
         <v>401</v>
@@ -20812,7 +20812,7 @@
         <v>459</v>
       </c>
       <c r="B656" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C656" s="4" t="s">
         <v>401</v>
@@ -20839,7 +20839,7 @@
         <v>460</v>
       </c>
       <c r="B657" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C657" s="4" t="s">
         <v>401</v>
@@ -20866,7 +20866,7 @@
         <v>461</v>
       </c>
       <c r="B658" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C658" s="4" t="s">
         <v>401</v>
@@ -20893,7 +20893,7 @@
         <v>462</v>
       </c>
       <c r="B659" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C659" s="4" t="s">
         <v>401</v>
@@ -20920,7 +20920,7 @@
         <v>463</v>
       </c>
       <c r="B660" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C660" s="4" t="s">
         <v>401</v>
@@ -20947,7 +20947,7 @@
         <v>464</v>
       </c>
       <c r="B661" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C661" s="4" t="s">
         <v>401</v>
@@ -20974,7 +20974,7 @@
         <v>465</v>
       </c>
       <c r="B662" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C662" s="4" t="s">
         <v>401</v>
@@ -21001,7 +21001,7 @@
         <v>466</v>
       </c>
       <c r="B663" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C663" s="4" t="s">
         <v>401</v>
@@ -21028,7 +21028,7 @@
         <v>467</v>
       </c>
       <c r="B664" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C664" s="4" t="s">
         <v>401</v>
@@ -21055,7 +21055,7 @@
         <v>468</v>
       </c>
       <c r="B665" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C665" s="4" t="s">
         <v>401</v>
@@ -21082,7 +21082,7 @@
         <v>469</v>
       </c>
       <c r="B666" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C666" s="4" t="s">
         <v>401</v>
@@ -21109,7 +21109,7 @@
         <v>470</v>
       </c>
       <c r="B667" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C667" s="4" t="s">
         <v>401</v>
@@ -21136,7 +21136,7 @@
         <v>471</v>
       </c>
       <c r="B668" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C668" s="4" t="s">
         <v>401</v>
@@ -21163,7 +21163,7 @@
         <v>463</v>
       </c>
       <c r="B669" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C669" s="4" t="s">
         <v>401</v>
@@ -21190,7 +21190,7 @@
         <v>472</v>
       </c>
       <c r="B670" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C670" s="4" t="s">
         <v>401</v>
@@ -21217,7 +21217,7 @@
         <v>464</v>
       </c>
       <c r="B671" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C671" s="4" t="s">
         <v>401</v>
@@ -21244,7 +21244,7 @@
         <v>465</v>
       </c>
       <c r="B672" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C672" s="4" t="s">
         <v>401</v>
@@ -21271,7 +21271,7 @@
         <v>466</v>
       </c>
       <c r="B673" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C673" s="4" t="s">
         <v>401</v>
@@ -21298,7 +21298,7 @@
         <v>473</v>
       </c>
       <c r="B674" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C674" s="4" t="s">
         <v>401</v>
@@ -21325,7 +21325,7 @@
         <v>468</v>
       </c>
       <c r="B675" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C675" s="4" t="s">
         <v>401</v>
@@ -21352,7 +21352,7 @@
         <v>469</v>
       </c>
       <c r="B676" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C676" s="4" t="s">
         <v>401</v>
@@ -21379,7 +21379,7 @@
         <v>470</v>
       </c>
       <c r="B677" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C677" s="4" t="s">
         <v>401</v>
@@ -21406,7 +21406,7 @@
         <v>474</v>
       </c>
       <c r="B678" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C678" s="4" t="s">
         <v>401</v>
@@ -21433,7 +21433,7 @@
         <v>475</v>
       </c>
       <c r="B679" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C679" s="4" t="s">
         <v>401</v>
@@ -21460,7 +21460,7 @@
         <v>464</v>
       </c>
       <c r="B680" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C680" s="4" t="s">
         <v>401</v>
@@ -21487,7 +21487,7 @@
         <v>476</v>
       </c>
       <c r="B681" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C681" s="4" t="s">
         <v>401</v>
@@ -21515,7 +21515,7 @@
         <v>477</v>
       </c>
       <c r="B682" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C682" s="4" t="s">
         <v>401</v>
@@ -21543,7 +21543,7 @@
         <v>478</v>
       </c>
       <c r="B683" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C683" s="4" t="s">
         <v>401</v>
@@ -21570,7 +21570,7 @@
         <v>467</v>
       </c>
       <c r="B684" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C684" s="4" t="s">
         <v>401</v>
@@ -21598,7 +21598,7 @@
         <v>468</v>
       </c>
       <c r="B685" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C685" s="4" t="s">
         <v>401</v>
@@ -21625,7 +21625,7 @@
         <v>469</v>
       </c>
       <c r="B686" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C686" s="4" t="s">
         <v>401</v>
@@ -21652,7 +21652,7 @@
         <v>470</v>
       </c>
       <c r="B687" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C687" s="4" t="s">
         <v>401</v>
@@ -21679,7 +21679,7 @@
         <v>474</v>
       </c>
       <c r="B688" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C688" s="4" t="s">
         <v>401</v>
@@ -21706,7 +21706,7 @@
         <v>475</v>
       </c>
       <c r="B689" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C689" s="4" t="s">
         <v>401</v>
@@ -21733,7 +21733,7 @@
         <v>479</v>
       </c>
       <c r="B690" s="4">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="C690" s="4" t="s">
         <v>401</v>

</xml_diff>